<commit_message>
update scrum doc formatting and doxygen comments
</commit_message>
<xml_diff>
--- a/MainWindow/SCRUM/CS1C_ERKK_Group_Project.xlsx
+++ b/MainWindow/SCRUM/CS1C_ERKK_Group_Project.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" state="visible" r:id="rId2"/>
@@ -1322,8 +1322,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3347,7 +3347,7 @@
   </sheetPr>
   <dimension ref="A1:AJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D42" activeCellId="0" sqref="D42"/>

</xml_diff>